<commit_message>
Deploying to gh-pages from  @ e05f264d84ccaa64d05c15d9d4c675f111a6568d 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/16.1.4.1a.xlsx
+++ b/en/downloads/data-excel/16.1.4.1a.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\korozbaeva\Desktop\ПоказателиЦУР для Платформы\Национальные показатели ЦУР\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\korozbaeva\Desktop\Показатели ЦУР для Платформы\Национальные показатели ЦУР\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -306,7 +306,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -400,6 +400,15 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -683,9 +692,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P14"/>
+  <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.25"/>
   <cols>
@@ -695,7 +706,7 @@
     <col min="4" max="16384" width="9.140625" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>34</v>
       </c>
@@ -706,7 +717,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>38</v>
       </c>
@@ -729,7 +740,7 @@
       <c r="N2" s="26"/>
       <c r="O2" s="28"/>
     </row>
-    <row r="3" spans="1:16" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="25"/>
       <c r="B3" s="29"/>
       <c r="C3" s="30"/>
@@ -746,7 +757,7 @@
       <c r="N3" s="26"/>
       <c r="O3" s="28"/>
     </row>
-    <row r="4" spans="1:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
@@ -795,8 +806,11 @@
       <c r="P4" s="8">
         <v>2019</v>
       </c>
+      <c r="Q4" s="8">
+        <v>2020</v>
+      </c>
     </row>
-    <row r="5" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>3</v>
       </c>
@@ -845,8 +859,11 @@
       <c r="P5" s="12">
         <v>8.5555715727259614</v>
       </c>
+      <c r="Q5" s="32">
+        <v>4.4631700362051845</v>
+      </c>
     </row>
-    <row r="6" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>6</v>
       </c>
@@ -895,8 +912,11 @@
       <c r="P6" s="16">
         <v>7.5607560756075607</v>
       </c>
+      <c r="Q6" s="33">
+        <v>22.107243650047039</v>
+      </c>
     </row>
-    <row r="7" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>9</v>
       </c>
@@ -945,8 +965,11 @@
       <c r="P7" s="16">
         <v>18.242710795902287</v>
       </c>
+      <c r="Q7" s="33">
+        <v>4.8469387755102042</v>
+      </c>
     </row>
-    <row r="8" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>12</v>
       </c>
@@ -995,8 +1018,11 @@
       <c r="P8" s="16">
         <v>10.464547677261614</v>
       </c>
+      <c r="Q8" s="33">
+        <v>11.270912826533607</v>
+      </c>
     </row>
-    <row r="9" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>15</v>
       </c>
@@ -1045,8 +1071,11 @@
       <c r="P9" s="16">
         <v>11.142322097378276</v>
       </c>
+      <c r="Q9" s="33">
+        <v>8.2663605051664764</v>
+      </c>
     </row>
-    <row r="10" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>18</v>
       </c>
@@ -1095,8 +1124,11 @@
       <c r="P10" s="16">
         <v>4.6357615894039732</v>
       </c>
+      <c r="Q10" s="33">
+        <v>9.0160381447767666</v>
+      </c>
     </row>
-    <row r="11" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>21</v>
       </c>
@@ -1145,8 +1177,11 @@
       <c r="P11" s="16">
         <v>21.302578018995931</v>
       </c>
+      <c r="Q11" s="33">
+        <v>2.7624309392265194</v>
+      </c>
     </row>
-    <row r="12" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>24</v>
       </c>
@@ -1195,8 +1230,11 @@
       <c r="P12" s="16">
         <v>4.9286498353457739</v>
       </c>
+      <c r="Q12" s="33">
+        <v>1.1408815903197926</v>
+      </c>
     </row>
-    <row r="13" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>27</v>
       </c>
@@ -1245,8 +1283,11 @@
       <c r="P13" s="16">
         <v>8.1795239744668216</v>
       </c>
+      <c r="Q13" s="33">
+        <v>1.7541111981205952</v>
+      </c>
     </row>
-    <row r="14" spans="1:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="19" t="s">
         <v>30</v>
       </c>
@@ -1294,6 +1335,9 @@
       </c>
       <c r="P14" s="22">
         <v>13.356461405030357</v>
+      </c>
+      <c r="Q14" s="34">
+        <v>3.6288232244686367</v>
       </c>
     </row>
   </sheetData>

</xml_diff>